<commit_message>
Updated production data for 2024
</commit_message>
<xml_diff>
--- a/data/tropical_fruit_production_value.xlsx
+++ b/data/tropical_fruit_production_value.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/Crop_production/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_943FE74C8EC581C5B2849BFBD14D0ACEAE597E59" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA58490F-4DEF-4888-8873-8DF017FE0DFE}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_943FE74C8EC581C5B2849BFBD14D0ACEAE597E59" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAAAC7C8-915E-44A3-9A3F-3ADF320419F9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="summary" sheetId="2" r:id="rId2"/>
+    <sheet name="2022-23" sheetId="3" r:id="rId1"/>
+    <sheet name="2020-21" sheetId="1" r:id="rId2"/>
+    <sheet name="summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="23">
   <si>
     <t>Crop</t>
   </si>
@@ -164,6 +165,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA4103DA-3AA9-4846-BCA8-A079D4CF2D9C}" name="Table12" displayName="Table12" ref="A1:D29" totalsRowShown="0">
+  <autoFilter ref="A1:D29" xr:uid="{B8267EE7-6FD8-4B4C-B409-0AD8BFD5CE76}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
+    <sortCondition ref="A1:A29"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FB5A6CDC-EAAB-4E4C-A93A-A397EF248671}" name="Crop"/>
+    <tableColumn id="2" xr3:uid="{02365875-B85C-4C76-BD39-54866C286D69}" name="State"/>
+    <tableColumn id="3" xr3:uid="{E9BD48B8-5054-4966-B0C3-A58E9EC383E9}" name="Yield"/>
+    <tableColumn id="4" xr3:uid="{E6C9DF19-6BC0-4A9B-B784-3275D3B2A87E}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B8267EE7-6FD8-4B4C-B409-0AD8BFD5CE76}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0">
   <autoFilter ref="A1:D29" xr:uid="{B8267EE7-6FD8-4B4C-B409-0AD8BFD5CE76}"/>
   <tableColumns count="4">
@@ -176,7 +193,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table5" displayName="Table5" ref="A1:C6" totalsRowShown="0">
   <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
@@ -189,9 +206,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +246,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -335,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -477,26 +494,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E85FB6-90CE-4820-9490-94FB9833FEBF}">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:M8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,331 +527,331 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>76035.91</v>
+        <v>42221.4</v>
       </c>
       <c r="D2" s="1">
-        <v>67163221.670000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99896326.670000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>30237.02</v>
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>158</v>
       </c>
       <c r="D3" s="1">
-        <v>203614505.53999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>402330.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>42221.4</v>
+        <v>18902.62</v>
       </c>
       <c r="D4" s="1">
-        <v>99896326.670000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <f>54771644.55+12229962.16</f>
+        <v>67001606.709999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>15580.5</v>
+        <v>1317.8</v>
       </c>
       <c r="D5" s="1">
-        <v>26690000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4223250.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
-        <v>2.34</v>
+        <v>3.2</v>
       </c>
       <c r="D6" s="1">
-        <v>2701.35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15394.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2314.85</v>
-      </c>
-      <c r="D7" s="1">
-        <v>13468914.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>158</v>
-      </c>
-      <c r="D8" s="1">
-        <v>402330.59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15580.5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>26690000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1272.76</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1124237.71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>1283.1000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2198000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
-        <v>18902.62</v>
+        <v>1466.4</v>
       </c>
       <c r="D12" s="1">
-        <f>54771644.55+12229962.16</f>
-        <v>67001606.709999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2512000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1283.1000000000001</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2198000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1">
-        <v>5648.05</v>
-      </c>
-      <c r="D15" s="1">
-        <v>42088393.880000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>1317.8</v>
+        <v>76035.91</v>
       </c>
       <c r="D16" s="1">
-        <v>4223250.46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67163221.670000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>1466.4</v>
+        <v>2.34</v>
       </c>
       <c r="D17" s="1">
-        <v>2512000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2701.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1272.76</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1124237.71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2937.95</v>
-      </c>
-      <c r="D19" s="1">
-        <v>21313422.199999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>15394.62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>11057.34</v>
+        <v>27646</v>
       </c>
       <c r="D23" s="1">
-        <v>66034274.369999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203614505.53999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2314.85</v>
+      </c>
+      <c r="D24" s="1">
+        <v>13468914.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5648.05</v>
+      </c>
+      <c r="D26" s="1">
+        <v>42088393.880000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1">
-        <v>6811.27</v>
+        <v>2937.95</v>
       </c>
       <c r="D27" s="1">
-        <v>40585493.109999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21313422.199999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1">
+        <v>11057.34</v>
+      </c>
+      <c r="D28" s="1">
+        <v>66034274.369999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
+      </c>
+      <c r="C29" s="1">
+        <v>6811.27</v>
+      </c>
+      <c r="D29" s="1">
+        <v>40585493.109999999</v>
       </c>
     </row>
   </sheetData>
@@ -847,77 +864,357 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>59006.48</v>
-      </c>
-      <c r="C2">
-        <v>387105003.19999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>76035.91</v>
+      </c>
+      <c r="D2" s="1">
+        <v>67163221.670000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>62603.02</v>
-      </c>
-      <c r="C3">
-        <v>171538909.05000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>30237.02</v>
+      </c>
+      <c r="D3" s="1">
+        <v>203614505.53999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>77311.009999999995</v>
-      </c>
-      <c r="C4">
-        <v>68290160.730000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42221.4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>99896326.670000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>16196</v>
-      </c>
-      <c r="C5">
-        <v>31400000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>15580.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>26690000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>215116.51</v>
-      </c>
-      <c r="C6">
-        <v>658334072.98000002</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2701.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2314.85</v>
+      </c>
+      <c r="D7" s="1">
+        <v>13468914.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>158</v>
+      </c>
+      <c r="D8" s="1">
+        <v>402330.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1272.76</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1124237.71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18902.62</v>
+      </c>
+      <c r="D12" s="1">
+        <f>54771644.55+12229962.16</f>
+        <v>67001606.709999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1283.1000000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2198000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5648.05</v>
+      </c>
+      <c r="D15" s="1">
+        <v>42088393.880000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1317.8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4223250.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1466.4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2512000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2937.95</v>
+      </c>
+      <c r="D19" s="1">
+        <v>21313422.199999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>15394.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1">
+        <v>11057.34</v>
+      </c>
+      <c r="D23" s="1">
+        <v>66034274.369999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1">
+        <v>6811.27</v>
+      </c>
+      <c r="D27" s="1">
+        <v>40585493.109999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -927,4 +1224,93 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>59006.48</v>
+      </c>
+      <c r="C2">
+        <v>387105003.19999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>62603.02</v>
+      </c>
+      <c r="C3">
+        <v>171538909.05000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>77311.009999999995</v>
+      </c>
+      <c r="C4">
+        <v>68290160.730000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>16196</v>
+      </c>
+      <c r="C5">
+        <v>31400000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>215116.51</v>
+      </c>
+      <c r="C6">
+        <v>658334072.98000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{adaa4be3-f650-4692-881a-64ae220cbceb}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update chickpea data 2024-25
</commit_message>
<xml_diff>
--- a/data/tropical_fruit_production_value.xlsx
+++ b/data/tropical_fruit_production_value.xlsx
@@ -8,7 +8,6 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/Crop_production/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_943FE74C8EC581C5B2849BFBD14D0ACEAE597E59" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAAAC7C8-915E-44A3-9A3F-3ADF320419F9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1310,7 +1309,5 @@
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{adaa4be3-f650-4692-881a-64ae220cbceb}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" removed="0"/>
-</clbl:labelList>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>